<commit_message>
funcexec and define functions overriding example is added
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-demo/src/main/resources/excel/define-funcexec/Modelexec_Test.xlsx
+++ b/calculation-engine/engine-demo/src/main/resources/excel/define-funcexec/Modelexec_Test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2250" windowWidth="22665" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="2700" windowWidth="22665" windowHeight="7680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -391,7 +391,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,7 +399,7 @@
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.7109375" customWidth="1"/>
     <col min="6" max="7" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
@@ -438,7 +438,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="e">
-        <f ca="1">DEFINE("DEF_1", F2, G2, "#", H2)</f>
+        <f ca="1">MODELDEFINE("DEF_1", F2, G2, "#", H2)</f>
         <v>#NAME?</v>
       </c>
       <c r="F2">

</xml_diff>